<commit_message>
deleted replicate xlsx sheets
</commit_message>
<xml_diff>
--- a/data/DS421_survey_responses.xlsx
+++ b/data/DS421_survey_responses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="5720" yWindow="5260" windowWidth="23080" windowHeight="12820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -4811,7 +4811,7 @@
   </sheetPr>
   <dimension ref="A1:FF18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -11797,7 +11797,7 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>